<commit_message>
added page with comments and added an initial architecture diagram
</commit_message>
<xml_diff>
--- a/sad/Study process table.xlsx
+++ b/sad/Study process table.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Learning and Development\general\softeq.education.general\sad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED6E62F-CF70-46E1-90A8-CC9E6CE0DAE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634F050B-D705-40AE-8568-FE52544C4613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{F38CD176-7B98-4C5D-96CA-2492731593CF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{F38CD176-7B98-4C5D-96CA-2492731593CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Goals" sheetId="2" r:id="rId1"/>
     <sheet name="Notes" sheetId="3" r:id="rId2"/>
     <sheet name="L&amp;D board" sheetId="1" r:id="rId3"/>
-    <sheet name="Лист4" sheetId="4" r:id="rId4"/>
+    <sheet name="Dev advises" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="159">
   <si>
     <t>Topic</t>
   </si>
@@ -453,6 +453,93 @@
   </si>
   <si>
     <t xml:space="preserve">Azure </t>
+  </si>
+  <si>
+    <t>Антон</t>
+  </si>
+  <si>
+    <t>Ориентироваться только на джунов</t>
+  </si>
+  <si>
+    <t>Делать задачки по базе</t>
+  </si>
+  <si>
+    <t>Устаревания документации сосредоточится только на базе</t>
+  </si>
+  <si>
+    <t>Глеб</t>
+  </si>
+  <si>
+    <t>смотрит PR дает задчки на уже существующий проект</t>
+  </si>
+  <si>
+    <t>Советы/критика/комментарии</t>
+  </si>
+  <si>
+    <t>Активность в обучении</t>
+  </si>
+  <si>
+    <t>Выполняет задачки делает PR, обучается</t>
+  </si>
+  <si>
+    <t>Нужные долгие задачи отбивают мотивацию учится</t>
+  </si>
+  <si>
+    <t>Небольшие но интересные задачи мотивируют</t>
+  </si>
+  <si>
+    <t>Дмитрий</t>
+  </si>
+  <si>
+    <t>Менторил Глеба изначально, предоставлял сведенье о первом проекте  изначальный проект</t>
+  </si>
+  <si>
+    <t>Идея  с стадиями и репозиториями понравилась</t>
+  </si>
+  <si>
+    <t>Думает хорошо бы если бы была заготовка проекта на React для тестирования</t>
+  </si>
+  <si>
+    <t>Святослав</t>
+  </si>
+  <si>
+    <t>Наполнял портал с задачами для джунов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Порталом не кто не пользуется </t>
+  </si>
+  <si>
+    <t>Можно попробовать на одном учебном проекте</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Для поддержки большой системы обучения требуется большая команда </t>
+  </si>
+  <si>
+    <t>Задачки вести относительно roadmap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Задачки вести относительно roadmap </t>
+  </si>
+  <si>
+    <t>https://github.com/MoienTajik/AspNetCore-Developer-Roadmap</t>
+  </si>
+  <si>
+    <t>Хорошо бы сделать портал с теорией и с сылками на рессурсы для обудения</t>
+  </si>
+  <si>
+    <t>Единый портал по которому вести всех джуниоров разработчиков</t>
+  </si>
+  <si>
+    <t>Хорошо бы заинтересновать в L&amp;D сеньоров (но это очень сложно)</t>
+  </si>
+  <si>
+    <t>Вышли на идеи обсуждать спорные топики на morning coffee</t>
+  </si>
+  <si>
+    <t>Нудные morning coffee</t>
+  </si>
+  <si>
+    <t>Найти баланс теории и практики, просто практикой не пользуются судя по предыдущему опыту</t>
   </si>
 </sst>
 </file>
@@ -537,7 +624,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -547,6 +634,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -564,7 +675,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -577,12 +688,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -901,7 +1031,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,7 +1111,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,7 +1228,7 @@
       <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1167,27 +1297,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D27B4423-E7EB-4F52-92BD-50C71A1C66CC}">
-  <dimension ref="A1:H100"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="67.7109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="38.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="89.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="113.7109375" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
@@ -1213,9 +1343,6 @@
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1228,9 +1355,6 @@
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
@@ -1242,9 +1366,6 @@
       <c r="A6" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D6" t="s">
-        <v>52</v>
-      </c>
       <c r="E6" s="1" t="s">
         <v>110</v>
       </c>
@@ -1259,9 +1380,6 @@
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D8" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
@@ -1271,111 +1389,157 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="D10" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D11" t="s">
+    </row>
+    <row r="12" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="19" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" s="20"/>
+    </row>
+    <row r="13" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="19" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" s="20"/>
+    </row>
+    <row r="14" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="19" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="E14" s="20"/>
+    </row>
+    <row r="15" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="B15" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="19" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="E15" s="20"/>
+    </row>
+    <row r="16" spans="1:8" s="12" customFormat="1" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
+      <c r="B16" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" s="19" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="21" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3" t="s">
+    <row r="17" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="17" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="3" t="s">
+      <c r="C17" s="18"/>
+      <c r="D17" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="20"/>
+    </row>
+    <row r="18" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="17" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="3" t="s">
+      <c r="C18" s="18"/>
+      <c r="D18" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="20"/>
+    </row>
+    <row r="19" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="17" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3" t="s">
+      <c r="C19" s="18"/>
+      <c r="D19" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="20"/>
+    </row>
+    <row r="20" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" s="17" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3" t="s">
+      <c r="C20" s="18"/>
+      <c r="D20" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="20"/>
+    </row>
+    <row r="21" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="B21" s="17" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="3" t="s">
+      <c r="C21" s="18"/>
+      <c r="D21" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="20"/>
+    </row>
+    <row r="22" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="B22" s="17" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="3" t="s">
+      <c r="C22" s="18"/>
+      <c r="D22" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="20"/>
+    </row>
+    <row r="23" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
+      <c r="B23" s="17" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="3" t="s">
+      <c r="C23" s="18"/>
+      <c r="D23" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="20"/>
+    </row>
+    <row r="24" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
+      <c r="B24" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="G24" t="s">
+      <c r="C24" s="18"/>
+      <c r="D24" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="20"/>
+      <c r="G24" s="13" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1399,47 +1563,45 @@
       <c r="A29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C34" s="4"/>
-      <c r="E34" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C35" s="4"/>
+      <c r="E35" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
-      <c r="B36" s="4"/>
+      <c r="B36" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="C36" s="4"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1448,120 +1610,122 @@
       <c r="C37" s="4"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="A38" s="2"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="A39" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39" s="4"/>
       <c r="C39" s="4"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="4"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C40" s="4"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="C41" s="4"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="2"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
-      <c r="B44" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
+      <c r="B45" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="2"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
-    </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="2"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
-      <c r="B49" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+      <c r="B52" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="2"/>
-      <c r="B53" s="3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
-      <c r="C54" s="3" t="s">
-        <v>69</v>
+      <c r="B54" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="C55" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="C56" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
-      <c r="B57" s="3" t="s">
-        <v>35</v>
+      <c r="C57" s="3" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
+      <c r="B58" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
@@ -1571,254 +1735,257 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
-      <c r="B61" s="3" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="2"/>
+      <c r="B63" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="2"/>
-      <c r="B64" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C64" s="5"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C65" s="5"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
-      <c r="B66" s="5"/>
+      <c r="B66" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="C66" s="5"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
+      <c r="A67" s="2"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="2"/>
-      <c r="B68" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
-      <c r="B69" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C69" s="5"/>
+      <c r="B69" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C70" s="5"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C71" s="5"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="2"/>
+      <c r="B72" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C71" s="5"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
+      <c r="C72" s="5"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="2"/>
-      <c r="B73" s="5" t="s">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="2"/>
+      <c r="B74" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C73" s="5"/>
-    </row>
-    <row r="74" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A74" s="2"/>
-      <c r="C74" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E74" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C74" s="5"/>
+    </row>
+    <row r="75" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="C75" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="C76" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="C77" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E77" t="s">
-        <v>95</v>
+        <v>87</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
+      <c r="C78" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E78" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
-      <c r="B79" s="3" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
-      <c r="C80" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E80" t="s">
-        <v>98</v>
+      <c r="B80" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="C81" s="3" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E81" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
-      <c r="B82" s="3" t="s">
-        <v>42</v>
+      <c r="C82" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E82" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
-      <c r="E83" t="s">
-        <v>101</v>
+      <c r="B83" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="E84" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="E85" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="E86" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="E87" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
-      <c r="B88" s="3" t="s">
-        <v>41</v>
+      <c r="E88" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
-      <c r="E89" t="s">
-        <v>100</v>
+      <c r="B89" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="E90" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="E91" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
-      <c r="B92" s="3" t="s">
-        <v>45</v>
+      <c r="E92" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
+      <c r="B99" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
+      <c r="A100" s="2"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
         <v>129</v>
       </c>
     </row>
@@ -1833,16 +2000,279 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A138A5A-9700-49AE-9668-53FAB1D07912}">
-  <dimension ref="E18"/>
+  <dimension ref="A1:AS29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16:M22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="89.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="87.5703125" customWidth="1"/>
+    <col min="4" max="4" width="37.28515625" style="20" customWidth="1"/>
+    <col min="5" max="45" width="9.140625" style="20"/>
+  </cols>
   <sheetData>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="12"/>
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A1" s="23"/>
+      <c r="B1" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:45" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="20"/>
+      <c r="V7" s="20"/>
+      <c r="W7" s="20"/>
+      <c r="X7" s="20"/>
+      <c r="Y7" s="20"/>
+      <c r="Z7" s="20"/>
+      <c r="AA7" s="20"/>
+      <c r="AB7" s="20"/>
+      <c r="AC7" s="20"/>
+      <c r="AD7" s="20"/>
+      <c r="AE7" s="20"/>
+      <c r="AF7" s="20"/>
+      <c r="AG7" s="20"/>
+      <c r="AH7" s="20"/>
+      <c r="AI7" s="20"/>
+      <c r="AJ7" s="20"/>
+      <c r="AK7" s="20"/>
+      <c r="AL7" s="20"/>
+      <c r="AM7" s="20"/>
+      <c r="AN7" s="20"/>
+      <c r="AO7" s="20"/>
+      <c r="AP7" s="20"/>
+      <c r="AQ7" s="20"/>
+      <c r="AR7" s="20"/>
+      <c r="AS7" s="20"/>
+    </row>
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:45" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="20"/>
+      <c r="U12" s="20"/>
+      <c r="V12" s="20"/>
+      <c r="W12" s="20"/>
+      <c r="X12" s="20"/>
+      <c r="Y12" s="20"/>
+      <c r="Z12" s="20"/>
+      <c r="AA12" s="20"/>
+      <c r="AB12" s="20"/>
+      <c r="AC12" s="20"/>
+      <c r="AD12" s="20"/>
+      <c r="AE12" s="20"/>
+      <c r="AF12" s="20"/>
+      <c r="AG12" s="20"/>
+      <c r="AH12" s="20"/>
+      <c r="AI12" s="20"/>
+      <c r="AJ12" s="20"/>
+      <c r="AK12" s="20"/>
+      <c r="AL12" s="20"/>
+      <c r="AM12" s="20"/>
+      <c r="AN12" s="20"/>
+      <c r="AO12" s="20"/>
+      <c r="AP12" s="20"/>
+      <c r="AQ12" s="20"/>
+      <c r="AR12" s="20"/>
+      <c r="AS12" s="20"/>
+    </row>
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:45" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="20"/>
+      <c r="T18" s="20"/>
+      <c r="U18" s="20"/>
+      <c r="V18" s="20"/>
+      <c r="W18" s="20"/>
+      <c r="X18" s="20"/>
+      <c r="Y18" s="20"/>
+      <c r="Z18" s="20"/>
+      <c r="AA18" s="20"/>
+      <c r="AB18" s="20"/>
+      <c r="AC18" s="20"/>
+      <c r="AD18" s="20"/>
+      <c r="AE18" s="20"/>
+      <c r="AF18" s="20"/>
+      <c r="AG18" s="20"/>
+      <c r="AH18" s="20"/>
+      <c r="AI18" s="20"/>
+      <c r="AJ18" s="20"/>
+      <c r="AK18" s="20"/>
+      <c r="AL18" s="20"/>
+      <c r="AM18" s="20"/>
+      <c r="AN18" s="20"/>
+      <c r="AO18" s="20"/>
+      <c r="AP18" s="20"/>
+      <c r="AQ18" s="20"/>
+      <c r="AR18" s="20"/>
+      <c r="AS18" s="20"/>
+    </row>
+    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>145</v>
+      </c>
+      <c r="B20" t="s">
+        <v>146</v>
+      </c>
+      <c r="C20" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>150</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="C27" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="E27" s="24"/>
+    </row>
+    <row r="28" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>158</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>